<commit_message>
added totals to some data
</commit_message>
<xml_diff>
--- a/data/extracted_data/raw_round2/data/Gaillard_etal_2024_Fig1.xlsx
+++ b/data/extracted_data/raw_round2/data/Gaillard_etal_2024_Fig1.xlsx
@@ -1,42 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d9723b3edd6c224/biotoxin_review/hab_depuration/data/extracted_data/raw_round2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/hab_depuration/data/extracted_data/raw_round2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{0DF19FB0-60A0-0946-BAED-201F003F8CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C35E550C-BF8E-8840-B8FB-C854E004F535}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B1D682-4AFA-C947-A240-3CE38382E06B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{E4055AB2-CCDE-2247-9B36-F1FB62CB34DB}"/>
+    <workbookView xWindow="2960" yWindow="500" windowWidth="20840" windowHeight="19520" xr2:uid="{E4055AB2-CCDE-2247-9B36-F1FB62CB34DB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$59</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="22">
   <si>
     <t>treatment</t>
   </si>
@@ -91,6 +87,18 @@
   <si>
     <t>*unclear depuration trend, assume the depuration starts at 6 hours</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of toxicity</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
@@ -125,8 +133,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,10 +163,578 @@
 </styleSheet>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Chris Free" refreshedDate="45972.463929398145" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="44" xr:uid="{1AF688D4-27EA-4340-BC08-B17640AEBA4F}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:F59" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="species" numFmtId="0">
+      <sharedItems count="3">
+        <s v="gill"/>
+        <s v="digestive gland"/>
+        <s v="remaining tissues"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="treatment" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="phase" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Uptake"/>
+        <s v="Depuration"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="day" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="6" maxValue="192" count="5">
+        <n v="6"/>
+        <n v="24"/>
+        <n v="96"/>
+        <n v="120"/>
+        <n v="192"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="toxicity" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.204778156996582" maxValue="506"/>
+    </cacheField>
+    <cacheField name="note" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="44">
+  <r>
+    <x v="0"/>
+    <s v="GDA"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="506"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDA"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="155.35714285714201"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="58.407079646017699"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="2.1238938053097298"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1.59292035398229"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDB"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="32.389380530973398"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDB"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="9.0265486725663493"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDB"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3.1858407079646098"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDC"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="20.707964601769898"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDC"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="7.4336283185840797"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDC"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2.1238938053097298"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDA-sa"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.2477876106194898"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDA-sa"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="7.4336283185840797"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="GDA-sa"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1.06194690265485"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="23.549488054607501"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="41.569965870307101"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="36.860068259385599"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1.02389078498293"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.204778156996582"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA-sa"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2.4573378839590401"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA-sa"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="9.4197952218430103"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA-sa"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="45.665529010238899"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA-sa"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="6.9624573378839596"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDA-sa"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1.4334470989761099"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 96 hours."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDB"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.8430034129692801"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDB"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2.0477815699658701"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDB"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1.22866894197953"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDC"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.4334470989761099"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDC"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.22866894197953"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="GDC"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1.63822525597269"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="131.92697768762599"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="23.829787234042499"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="8.2978723404255206"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1.27659574468086"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1.4893617021276599"/>
+    <s v="*The paper identified that depuration begins at 120 hours; however, toxicity shows a decline as early as 6 hours."/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDB"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.59574468085105"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDB"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.27659574468086"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDB"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.21276595744680499"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDC"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.6808510638297998"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDC"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.63829787234041602"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDC"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.21276595744680499"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA-sa"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2.5531914893616898"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA-sa"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.4893617021276599"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="GDA-sa"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.21276595744680499"/>
+    <s v="*unclear depuration trend, assume the depuration starts at 6 hours"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD22F8A5-23FA-8B4A-AA86-3C000240941D}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="0"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="25">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of toxicity" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +772,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -291,7 +878,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,7 +1020,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,16 +1028,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F6BED1-3AA0-E54E-AC48-A3163BCA1070}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="3" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -481,7 +1071,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -501,7 +1091,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>24</v>
@@ -581,7 +1171,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -601,7 +1191,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>24</v>
@@ -638,19 +1228,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="E10">
-        <v>20.707964601769898</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -658,19 +1245,16 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="E11">
-        <v>7.4336283185840797</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -681,13 +1265,13 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="E12">
-        <v>2.1238938053097298</v>
+        <v>20.707964601769898</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -698,16 +1282,16 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E13">
-        <v>4.2477876106194898</v>
+        <v>7.4336283185840797</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -718,16 +1302,16 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E14">
-        <v>7.4336283185840797</v>
+        <v>2.1238938053097298</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
@@ -738,139 +1322,127 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="E15">
-        <v>1.06194690265485</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="E16">
-        <v>23.549488054607501</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>41.569965870307101</v>
+        <v>4.2477876106194898</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E18">
-        <v>36.860068259385599</v>
+        <v>7.4336283185840797</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
       <c r="D19">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E19">
-        <v>1.02389078498293</v>
+        <v>1.06194690265485</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
       </c>
       <c r="D20">
+        <v>120</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
         <v>192</v>
       </c>
-      <c r="E20">
-        <v>0.204778156996582</v>
-      </c>
-      <c r="F20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
       <c r="E21">
-        <v>2.4573378839590401</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -878,16 +1450,16 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E22">
-        <v>9.4197952218430103</v>
+        <v>23.549488054607501</v>
       </c>
       <c r="F22" t="s">
         <v>16</v>
@@ -898,16 +1470,16 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E23">
-        <v>45.665529010238899</v>
+        <v>41.569965870307101</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
@@ -918,16 +1490,16 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
       </c>
       <c r="D24">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E24">
-        <v>6.9624573378839596</v>
+        <v>36.860068259385599</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
@@ -938,16 +1510,16 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
       </c>
       <c r="D25">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="E25">
-        <v>1.4334470989761099</v>
+        <v>1.02389078498293</v>
       </c>
       <c r="F25" t="s">
         <v>16</v>
@@ -958,19 +1530,19 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="E26">
-        <v>1.8430034129692801</v>
+        <v>0.204778156996582</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -978,19 +1550,19 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E27">
-        <v>2.0477815699658701</v>
+        <v>2.4573378839590401</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -998,19 +1570,19 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E28">
-        <v>1.22866894197953</v>
+        <v>9.4197952218430103</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1018,19 +1590,19 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="E29">
-        <v>1.4334470989761099</v>
+        <v>45.665529010238899</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1038,19 +1610,19 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
       </c>
       <c r="D30">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="E30">
-        <v>1.22866894197953</v>
+        <v>6.9624573378839596</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1058,67 +1630,67 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>13</v>
       </c>
       <c r="D31">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="E31">
-        <v>1.63822525597269</v>
+        <v>1.4334470989761099</v>
       </c>
       <c r="F31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>6</v>
       </c>
       <c r="E32">
-        <v>131.92697768762599</v>
+        <v>1.8430034129692801</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33">
         <v>24</v>
       </c>
       <c r="E33">
-        <v>23.829787234042499</v>
+        <v>2.0477815699658701</v>
       </c>
       <c r="F33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
@@ -1127,18 +1699,18 @@
         <v>96</v>
       </c>
       <c r="E34">
-        <v>8.2978723404255206</v>
+        <v>1.22866894197953</v>
       </c>
       <c r="F34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
@@ -1147,18 +1719,15 @@
         <v>120</v>
       </c>
       <c r="E35">
-        <v>1.27659574468086</v>
-      </c>
-      <c r="F35" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
@@ -1167,27 +1736,24 @@
         <v>192</v>
       </c>
       <c r="E36">
-        <v>1.4893617021276599</v>
-      </c>
-      <c r="F36" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37">
         <v>6</v>
       </c>
       <c r="E37">
-        <v>6.59574468085105</v>
+        <v>1.4334470989761099</v>
       </c>
       <c r="F37" t="s">
         <v>17</v>
@@ -1195,19 +1761,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38">
         <v>24</v>
       </c>
       <c r="E38">
-        <v>1.27659574468086</v>
+        <v>1.22866894197953</v>
       </c>
       <c r="F38" t="s">
         <v>17</v>
@@ -1215,10 +1781,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
@@ -1227,7 +1793,7 @@
         <v>96</v>
       </c>
       <c r="E39">
-        <v>0.21276595744680499</v>
+        <v>1.63822525597269</v>
       </c>
       <c r="F39" t="s">
         <v>17</v>
@@ -1235,7 +1801,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -1244,18 +1810,15 @@
         <v>13</v>
       </c>
       <c r="D40">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="E40">
-        <v>4.6808510638297998</v>
-      </c>
-      <c r="F40" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
@@ -1264,13 +1827,10 @@
         <v>13</v>
       </c>
       <c r="D41">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="E41">
-        <v>0.63829787234041602</v>
-      </c>
-      <c r="F41" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1278,19 +1838,19 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="E42">
-        <v>0.21276595744680499</v>
+        <v>131.92697768762599</v>
       </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1298,19 +1858,19 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E43">
-        <v>2.5531914893616898</v>
+        <v>23.829787234042499</v>
       </c>
       <c r="F43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1318,19 +1878,19 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
       </c>
       <c r="D44">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E44">
-        <v>1.4893617021276599</v>
+        <v>8.2978723404255206</v>
       </c>
       <c r="F44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1338,23 +1898,1052 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
         <v>13</v>
       </c>
       <c r="D45">
+        <v>120</v>
+      </c>
+      <c r="E45">
+        <v>1.27659574468086</v>
+      </c>
+      <c r="F45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46">
+        <v>192</v>
+      </c>
+      <c r="E46">
+        <v>1.4893617021276599</v>
+      </c>
+      <c r="F46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>6.59574468085105</v>
+      </c>
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48">
+        <v>24</v>
+      </c>
+      <c r="E48">
+        <v>1.27659574468086</v>
+      </c>
+      <c r="F48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
         <v>96</v>
       </c>
-      <c r="E45">
+      <c r="E49">
         <v>0.21276595744680499</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F49" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>120</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51">
+        <v>192</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>4.6808510638297998</v>
+      </c>
+      <c r="F52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <v>24</v>
+      </c>
+      <c r="E53">
+        <v>0.63829787234041602</v>
+      </c>
+      <c r="F53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54">
+        <v>96</v>
+      </c>
+      <c r="E54">
+        <v>0.21276595744680499</v>
+      </c>
+      <c r="F54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>120</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56">
+        <v>192</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>2.5531914893616898</v>
+      </c>
+      <c r="F57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58">
+        <v>24</v>
+      </c>
+      <c r="E58">
+        <v>1.4893617021276599</v>
+      </c>
+      <c r="F58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59">
+        <v>96</v>
+      </c>
+      <c r="E59">
+        <v>0.21276595744680499</v>
+      </c>
+      <c r="F59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60">
+        <v>120</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61">
+        <v>192</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62">
+        <v>6</v>
+      </c>
+      <c r="E62" s="3">
+        <v>29.283276450511934</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63">
+        <v>24</v>
+      </c>
+      <c r="E63" s="3">
+        <v>54.26621160409551</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64">
+        <v>96</v>
+      </c>
+      <c r="E64" s="3">
+        <v>85.392491467576718</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65">
+        <v>120</v>
+      </c>
+      <c r="E65" s="3">
+        <v>7.9863481228668896</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66">
+        <v>192</v>
+      </c>
+      <c r="E66" s="3">
+        <v>1.638225255972692</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>6</v>
+      </c>
+      <c r="E67" s="3">
+        <v>563.3451327433628</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68">
+        <v>24</v>
+      </c>
+      <c r="E68" s="3">
+        <v>179.25094816687653</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69">
+        <v>96</v>
+      </c>
+      <c r="E69" s="3">
+        <v>64.778761061946881</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70">
+        <v>120</v>
+      </c>
+      <c r="E70" s="3">
+        <v>2.1238938053097298</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71">
+        <v>192</v>
+      </c>
+      <c r="E71" s="3">
+        <v>1.59292035398229</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72">
+        <v>6</v>
+      </c>
+      <c r="E72" s="3">
+        <v>145.75676492166855</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73">
+        <v>24</v>
+      </c>
+      <c r="E73" s="3">
+        <v>27.234042553191436</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74">
+        <v>96</v>
+      </c>
+      <c r="E74" s="3">
+        <v>8.936170212765937</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75">
+        <v>120</v>
+      </c>
+      <c r="E75" s="3">
+        <v>1.27659574468086</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76">
+        <v>192</v>
+      </c>
+      <c r="E76" s="3">
+        <v>1.4893617021276599</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F59" xr:uid="{0EF51C61-6A8F-EE45-A402-E9403F353AF4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E25AC9-7543-3A44-80D6-E22CE19B3659}">
+  <dimension ref="A3:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>95.017064846416289</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3">
+        <v>29.283276450511934</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>96</v>
+      </c>
+      <c r="B6" s="3">
+        <v>85.392491467576718</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="5">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3">
+        <v>54.26621160409551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>120</v>
+      </c>
+      <c r="B7" s="3">
+        <v>7.9863481228668896</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="5">
+        <v>96</v>
+      </c>
+      <c r="I7" s="3">
+        <v>85.392491467576718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>192</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.638225255972692</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="5">
+        <v>120</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7.9863481228668896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3">
+        <v>83.549488054607451</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="5">
+        <v>192</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.638225255972692</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <v>29.283276450511934</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <v>563.3451327433628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3">
+        <v>54.26621160409551</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="5">
+        <v>24</v>
+      </c>
+      <c r="I11" s="3">
+        <v>179.25094816687653</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="5">
+        <v>96</v>
+      </c>
+      <c r="I12" s="3">
+        <v>64.778761061946881</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>68.495575221238909</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="5">
+        <v>120</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2.1238938053097298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>96</v>
+      </c>
+      <c r="B14" s="3">
+        <v>64.778761061946881</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="5">
+        <v>192</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.59292035398229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>120</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2.1238938053097298</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="5">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3">
+        <v>145.75676492166855</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>192</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.59292035398229</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="5">
+        <v>24</v>
+      </c>
+      <c r="I16" s="3">
+        <v>27.234042553191436</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3">
+        <v>742.59608091023938</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="5">
+        <v>96</v>
+      </c>
+      <c r="I17" s="3">
+        <v>8.936170212765937</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3">
+        <v>563.3451327433628</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="5">
+        <v>120</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1.27659574468086</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3">
+        <v>179.25094816687653</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="5">
+        <v>192</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1.4893617021276599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3">
+        <v>11.702127659574456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>96</v>
+      </c>
+      <c r="B22" s="3">
+        <v>8.936170212765937</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>120</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1.27659574468086</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>192</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.4893617021276599</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3">
+        <v>172.99080747485999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>6</v>
+      </c>
+      <c r="B26" s="3">
+        <v>145.75676492166855</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3">
+        <v>27.234042553191436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1174.3511441669361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>